<commit_message>
Finsihed a2, final results taken
</commit_message>
<xml_diff>
--- a/a2/part2/RMITGP/results.xlsx
+++ b/a2/part2/RMITGP/results.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\comp307\a2\part2\com\RMITGP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\monterey.ecs.vuw.ac.nz\dobbiedavi\Documents\comp307\a2\part2\RMITGP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15750" windowHeight="21300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="8055"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1582,8 +1582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1954,7 +1954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>

</xml_diff>